<commit_message>
Update for lecture 2018
</commit_message>
<xml_diff>
--- a/assets/example_6_1.xlsx
+++ b/assets/example_6_1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alchemyst/Documents/Development/control_notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alchemyst/Documents/Development/control_notebooks/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2446F5FD-9CE4-CA47-8CA4-3E28B1E7CC70}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -84,12 +85,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -103,7 +107,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Linear regression</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -175,6 +203,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.314036202876875"/>
+                  <c:y val="-2.3822149959813042E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
@@ -182,19 +260,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.8</c:v>
@@ -209,7 +287,7 @@
                   <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -221,10 +299,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.4</c:v>
@@ -254,6 +332,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6148-F44E-AD45-F6FA1099ED94}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -287,6 +370,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fuel Flow Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -348,6 +487,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power Generated</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1006,7 +1201,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1286,11 +1487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,6 +1590,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>